<commit_message>
Added stack code in test case - Gmail
</commit_message>
<xml_diff>
--- a/DSSTestAutomationFramework1.2/EmailIDTestData.xlsx
+++ b/DSSTestAutomationFramework1.2/EmailIDTestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14460" windowHeight="6270" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14460" windowHeight="5535" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="AOL" sheetId="7" r:id="rId1"/>
@@ -14,7 +14,7 @@
     <sheet name="Facebook" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="A1:M18"/>
+  <oleSize ref="A1:M16"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="16">
   <si>
     <t>Password</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>aa@facbook.com</t>
+  </si>
+  <si>
+    <t>tribune1</t>
+  </si>
+  <si>
+    <t>tribunedss@gmail.com</t>
+  </si>
+  <si>
+    <t>jamesmillerfacbook@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -128,11 +137,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -651,13 +663,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="1" max="1" width="34.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -701,25 +713,26 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>2</v>
+      <c r="A6" s="4" t="s">
+        <v>15</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="A3:A7" r:id="rId2" display="aa@gmail.com"/>
+    <hyperlink ref="A7" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -729,7 +742,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>

</xml_diff>